<commit_message>
Added avg percent change per year columns to data
</commit_message>
<xml_diff>
--- a/Simulation & Risk/Data/Analysis_Data.xlsx
+++ b/Simulation & Risk/Data/Analysis_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adlabarr\Google Drive\IAA\Courses\IAA\Simulation and Risk\Homework\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Desktop\IAA\Spring 1\spring1-orange5\Simulation &amp; Risk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9C3C89-22BF-4998-AC44-FDCF3A7D2DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Projections" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,22 @@
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>High Oil Price</t>
   </si>
@@ -90,11 +101,17 @@
   <si>
     <t>Arithmetic Return - Dry Well</t>
   </si>
+  <si>
+    <t>Average Cost per year</t>
+  </si>
+  <si>
+    <t>Arithmetic average return</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy"/>
   </numFmts>
@@ -261,7 +278,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -296,12 +313,18 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="3"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,6 +415,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -427,6 +467,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -602,7 +659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D34"/>
   <sheetViews>
@@ -610,20 +667,20 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.59765625" customWidth="1"/>
-    <col min="3" max="3" width="16.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="18"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -633,7 +690,7 @@
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -647,7 +704,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2020</v>
       </c>
@@ -661,7 +718,7 @@
         <v>62.993518999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>2021</v>
       </c>
@@ -675,7 +732,7 @@
         <v>69.901413000000005</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2022</v>
       </c>
@@ -689,7 +746,7 @@
         <v>72.684676999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>2023</v>
       </c>
@@ -703,7 +760,7 @@
         <v>74.801017999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>2024</v>
       </c>
@@ -717,7 +774,7 @@
         <v>75.938805000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>2025</v>
       </c>
@@ -731,7 +788,7 @@
         <v>77.019867000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>2026</v>
       </c>
@@ -745,7 +802,7 @@
         <v>77.178398000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>2027</v>
       </c>
@@ -759,7 +816,7 @@
         <v>77.449477999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>2028</v>
       </c>
@@ -773,7 +830,7 @@
         <v>78.719161999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>2029</v>
       </c>
@@ -787,7 +844,7 @@
         <v>80.201019000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>2030</v>
       </c>
@@ -801,7 +858,7 @@
         <v>81.341544999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>2031</v>
       </c>
@@ -815,7 +872,7 @@
         <v>82.912018000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>2032</v>
       </c>
@@ -829,7 +886,7 @@
         <v>84.124129999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>2033</v>
       </c>
@@ -843,7 +900,7 @@
         <v>85.351967000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>2034</v>
       </c>
@@ -857,7 +914,7 @@
         <v>86.263489000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>2035</v>
       </c>
@@ -871,7 +928,7 @@
         <v>87.272407999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>2036</v>
       </c>
@@ -885,7 +942,7 @@
         <v>87.882683</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>2037</v>
       </c>
@@ -899,7 +956,7 @@
         <v>89.997146999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>2038</v>
       </c>
@@ -913,7 +970,7 @@
         <v>91.438621999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>2039</v>
       </c>
@@ -927,7 +984,7 @@
         <v>92.675017999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>2040</v>
       </c>
@@ -941,7 +998,7 @@
         <v>93.648635999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>2041</v>
       </c>
@@ -955,7 +1012,7 @@
         <v>94.775542999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>2042</v>
       </c>
@@ -969,7 +1026,7 @@
         <v>95.301627999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>2043</v>
       </c>
@@ -983,7 +1040,7 @@
         <v>95.840835999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>2044</v>
       </c>
@@ -997,7 +1054,7 @@
         <v>96.296463000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>2045</v>
       </c>
@@ -1011,7 +1068,7 @@
         <v>96.973877000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>2046</v>
       </c>
@@ -1025,7 +1082,7 @@
         <v>96.859229999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>2047</v>
       </c>
@@ -1039,7 +1096,7 @@
         <v>97.643196000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>2048</v>
       </c>
@@ -1053,7 +1110,7 @@
         <v>98.581688</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>2049</v>
       </c>
@@ -1067,7 +1124,7 @@
         <v>99.111778000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>2050</v>
       </c>
@@ -1086,33 +1143,35 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" customWidth="1"/>
-    <col min="2" max="7" width="27.73046875" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="5" width="27.77734375" customWidth="1"/>
+    <col min="6" max="6" width="27.77734375" style="16" customWidth="1"/>
+    <col min="7" max="9" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
@@ -1124,8 +1183,10 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
-    </row>
-    <row r="3" spans="1:7" ht="40.15" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
@@ -1139,16 +1200,22 @@
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>22097</v>
       </c>
@@ -1161,17 +1228,22 @@
       <c r="D4" s="11">
         <v>44</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
+      <c r="E4" s="20">
+        <f t="shared" ref="E4:E34" si="0">SUM(B4:D4)/3</f>
+        <v>66.3</v>
+      </c>
+      <c r="F4" s="22"/>
       <c r="G4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>22462</v>
       </c>
@@ -1184,20 +1256,28 @@
       <c r="D5" s="13">
         <v>45.2</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="20">
+        <f t="shared" si="0"/>
+        <v>63.733333333333327</v>
+      </c>
+      <c r="F5" s="23">
+        <f t="shared" ref="F5:F35" si="1">(E5-E4)/E4</f>
+        <v>-3.8712921065862292E-2</v>
+      </c>
+      <c r="G5" s="16">
         <f>(B5-B4)/B4</f>
         <v>-1.7241379310344935E-2</v>
       </c>
-      <c r="F5" s="16">
-        <f t="shared" ref="F5:G5" si="0">(C5-C4)/C4</f>
+      <c r="H5" s="16">
+        <f t="shared" ref="H5:I5" si="2">(C5-C4)/C4</f>
         <v>-7.7896786757546244E-2</v>
       </c>
-      <c r="G5" s="16">
-        <f t="shared" si="0"/>
+      <c r="I5" s="16">
+        <f t="shared" si="2"/>
         <v>2.7272727272727337E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>22827</v>
       </c>
@@ -1210,20 +1290,28 @@
       <c r="D6" s="14">
         <v>50.8</v>
       </c>
-      <c r="E6" s="16">
-        <f t="shared" ref="E6:E51" si="1">(B6-B5)/B5</f>
+      <c r="E6" s="20">
+        <f t="shared" si="0"/>
+        <v>67.366666666666674</v>
+      </c>
+      <c r="F6" s="23">
+        <f t="shared" si="1"/>
+        <v>5.7008368200837038E-2</v>
+      </c>
+      <c r="G6" s="16">
+        <f t="shared" ref="G6:G51" si="3">(B6-B5)/B5</f>
         <v>5.6530214424951382E-2</v>
       </c>
-      <c r="F6" s="16">
-        <f t="shared" ref="F6:F51" si="2">(C6-C5)/C5</f>
+      <c r="H6" s="16">
+        <f t="shared" ref="H6:H51" si="4">(C6-C5)/C5</f>
         <v>2.5343189017951333E-2</v>
       </c>
-      <c r="G6" s="16">
-        <f t="shared" ref="G6:G51" si="3">(D6-D5)/D5</f>
+      <c r="I6" s="16">
+        <f t="shared" ref="I6:I51" si="5">(D6-D5)/D5</f>
         <v>0.12389380530973439</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>23192</v>
       </c>
@@ -1236,20 +1324,28 @@
       <c r="D7" s="13">
         <v>48.2</v>
       </c>
-      <c r="E7" s="16">
-        <f t="shared" si="1"/>
+      <c r="E7" s="20">
+        <f t="shared" si="0"/>
+        <v>64.133333333333326</v>
+      </c>
+      <c r="F7" s="23">
+        <f t="shared" si="1"/>
+        <v>-4.7996041563582607E-2</v>
+      </c>
+      <c r="G7" s="16">
+        <f t="shared" si="3"/>
         <v>-4.4280442804428145E-2</v>
       </c>
-      <c r="F7" s="16">
-        <f t="shared" si="2"/>
+      <c r="H7" s="16">
+        <f t="shared" si="4"/>
         <v>-4.8403707518022546E-2</v>
       </c>
-      <c r="G7" s="16">
-        <f t="shared" si="3"/>
+      <c r="I7" s="16">
+        <f t="shared" si="5"/>
         <v>-5.1181102362204613E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>23558</v>
       </c>
@@ -1262,20 +1358,28 @@
       <c r="D8" s="14">
         <v>48.5</v>
       </c>
-      <c r="E8" s="16">
-        <f t="shared" si="1"/>
+      <c r="E8" s="20">
+        <f t="shared" si="0"/>
+        <v>67.966666666666669</v>
+      </c>
+      <c r="F8" s="23">
+        <f t="shared" si="1"/>
+        <v>5.9771309771309927E-2</v>
+      </c>
+      <c r="G8" s="16">
+        <f t="shared" si="3"/>
         <v>-2.3166023166023085E-2</v>
       </c>
-      <c r="F8" s="16">
-        <f t="shared" si="2"/>
+      <c r="H8" s="16">
+        <f t="shared" si="4"/>
         <v>0.1341991341991341</v>
       </c>
-      <c r="G8" s="16">
-        <f t="shared" si="3"/>
+      <c r="I8" s="16">
+        <f t="shared" si="5"/>
         <v>6.2240663900414344E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>23923</v>
       </c>
@@ -1288,20 +1392,28 @@
       <c r="D9" s="13">
         <v>53.1</v>
       </c>
-      <c r="E9" s="16">
-        <f t="shared" si="1"/>
+      <c r="E9" s="20">
+        <f t="shared" si="0"/>
+        <v>70.533333333333331</v>
+      </c>
+      <c r="F9" s="23">
+        <f t="shared" si="1"/>
+        <v>3.7763609612555114E-2</v>
+      </c>
+      <c r="G9" s="16">
+        <f t="shared" si="3"/>
         <v>0.11857707509881422</v>
       </c>
-      <c r="F9" s="16">
-        <f t="shared" si="2"/>
+      <c r="H9" s="16">
+        <f t="shared" si="4"/>
         <v>-2.7671755725190757E-2</v>
       </c>
-      <c r="G9" s="16">
-        <f t="shared" si="3"/>
+      <c r="I9" s="16">
+        <f t="shared" si="5"/>
         <v>9.4845360824742292E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>24288</v>
       </c>
@@ -1314,20 +1426,28 @@
       <c r="D10" s="14">
         <v>56.9</v>
       </c>
-      <c r="E10" s="16">
-        <f t="shared" si="1"/>
+      <c r="E10" s="20">
+        <f t="shared" si="0"/>
+        <v>84.3</v>
+      </c>
+      <c r="F10" s="23">
+        <f t="shared" si="1"/>
+        <v>0.19517958412098299</v>
+      </c>
+      <c r="G10" s="16">
+        <f t="shared" si="3"/>
         <v>9.8939929328621931E-2</v>
       </c>
-      <c r="F10" s="16">
-        <f t="shared" si="2"/>
+      <c r="H10" s="16">
+        <f t="shared" si="4"/>
         <v>0.31305201177625125</v>
       </c>
-      <c r="G10" s="16">
-        <f t="shared" si="3"/>
+      <c r="I10" s="16">
+        <f t="shared" si="5"/>
         <v>7.1563088512240997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>24653</v>
       </c>
@@ -1340,20 +1460,28 @@
       <c r="D11" s="13">
         <v>61.5</v>
       </c>
-      <c r="E11" s="16">
-        <f t="shared" si="1"/>
+      <c r="E11" s="20">
+        <f t="shared" si="0"/>
+        <v>89.7</v>
+      </c>
+      <c r="F11" s="23">
+        <f t="shared" si="1"/>
+        <v>6.4056939501779431E-2</v>
+      </c>
+      <c r="G11" s="16">
+        <f t="shared" si="3"/>
         <v>7.0739549839228158E-2</v>
       </c>
-      <c r="F11" s="16">
-        <f t="shared" si="2"/>
+      <c r="H11" s="16">
+        <f t="shared" si="4"/>
         <v>5.3811659192825025E-2</v>
       </c>
-      <c r="G11" s="16">
-        <f t="shared" si="3"/>
+      <c r="I11" s="16">
+        <f t="shared" si="5"/>
         <v>8.0843585237258375E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>25019</v>
       </c>
@@ -1366,20 +1494,28 @@
       <c r="D12" s="14">
         <v>66.2</v>
       </c>
-      <c r="E12" s="16">
-        <f t="shared" si="1"/>
+      <c r="E12" s="20">
+        <f t="shared" si="0"/>
+        <v>97.933333333333337</v>
+      </c>
+      <c r="F12" s="23">
+        <f t="shared" si="1"/>
+        <v>9.1787439613526575E-2</v>
+      </c>
+      <c r="G12" s="16">
+        <f t="shared" si="3"/>
         <v>0.1876876876876877</v>
       </c>
-      <c r="F12" s="16">
-        <f t="shared" si="2"/>
+      <c r="H12" s="16">
+        <f t="shared" si="4"/>
         <v>5.3191489361702128E-2</v>
       </c>
-      <c r="G12" s="16">
-        <f t="shared" si="3"/>
+      <c r="I12" s="16">
+        <f t="shared" si="5"/>
         <v>7.6422764227642326E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>25384</v>
       </c>
@@ -1392,20 +1528,28 @@
       <c r="D13" s="13">
         <v>70.2</v>
       </c>
-      <c r="E13" s="16">
-        <f t="shared" si="1"/>
+      <c r="E13" s="20">
+        <f t="shared" si="0"/>
+        <v>103.66666666666667</v>
+      </c>
+      <c r="F13" s="23">
+        <f t="shared" si="1"/>
+        <v>5.8543226684819615E-2</v>
+      </c>
+      <c r="G13" s="16">
+        <f t="shared" si="3"/>
         <v>9.3552465233881235E-2</v>
       </c>
-      <c r="F13" s="16">
-        <f t="shared" si="2"/>
+      <c r="H13" s="16">
+        <f t="shared" si="4"/>
         <v>3.9057239057239131E-2</v>
       </c>
-      <c r="G13" s="16">
-        <f t="shared" si="3"/>
+      <c r="I13" s="16">
+        <f t="shared" si="5"/>
         <v>6.0422960725075525E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>25749</v>
       </c>
@@ -1418,20 +1562,28 @@
       <c r="D14" s="14">
         <v>80.900000000000006</v>
       </c>
-      <c r="E14" s="16">
-        <f t="shared" si="1"/>
+      <c r="E14" s="20">
+        <f t="shared" si="0"/>
+        <v>109.43333333333332</v>
+      </c>
+      <c r="F14" s="23">
+        <f t="shared" si="1"/>
+        <v>5.56270096463021E-2</v>
+      </c>
+      <c r="G14" s="16">
+        <f t="shared" si="3"/>
         <v>2.3121387283237321E-3</v>
       </c>
-      <c r="F14" s="16">
-        <f t="shared" si="2"/>
+      <c r="H14" s="16">
+        <f t="shared" si="4"/>
         <v>4.1477640959170295E-2</v>
       </c>
-      <c r="G14" s="16">
-        <f t="shared" si="3"/>
+      <c r="I14" s="16">
+        <f t="shared" si="5"/>
         <v>0.15242165242165245</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>26114</v>
       </c>
@@ -1444,20 +1596,28 @@
       <c r="D15" s="13">
         <v>86.8</v>
       </c>
-      <c r="E15" s="16">
-        <f t="shared" si="1"/>
+      <c r="E15" s="20">
+        <f t="shared" si="0"/>
+        <v>110.60000000000001</v>
+      </c>
+      <c r="F15" s="23">
+        <f t="shared" si="1"/>
+        <v>1.0660980810234717E-2</v>
+      </c>
+      <c r="G15" s="16">
+        <f t="shared" si="3"/>
         <v>-9.5732410611303304E-2</v>
       </c>
-      <c r="F15" s="16">
-        <f t="shared" si="2"/>
+      <c r="H15" s="16">
+        <f t="shared" si="4"/>
         <v>3.6714374611076579E-2</v>
       </c>
-      <c r="G15" s="16">
-        <f t="shared" si="3"/>
+      <c r="I15" s="16">
+        <f t="shared" si="5"/>
         <v>7.292954264524093E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>26480</v>
       </c>
@@ -1470,20 +1630,28 @@
       <c r="D16" s="14">
         <v>94.9</v>
       </c>
-      <c r="E16" s="16">
-        <f t="shared" si="1"/>
+      <c r="E16" s="20">
+        <f t="shared" si="0"/>
+        <v>115.40000000000002</v>
+      </c>
+      <c r="F16" s="23">
+        <f t="shared" si="1"/>
+        <v>4.3399638336347295E-2</v>
+      </c>
+      <c r="G16" s="16">
+        <f t="shared" si="3"/>
         <v>0.19260204081632645</v>
       </c>
-      <c r="F16" s="16">
-        <f t="shared" si="2"/>
+      <c r="H16" s="16">
+        <f t="shared" si="4"/>
         <v>-5.2821128451380449E-2</v>
       </c>
-      <c r="G16" s="16">
-        <f t="shared" si="3"/>
+      <c r="I16" s="16">
+        <f t="shared" si="5"/>
         <v>9.331797235023051E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>26845</v>
       </c>
@@ -1496,20 +1664,28 @@
       <c r="D17" s="13">
         <v>105.8</v>
       </c>
-      <c r="E17" s="16">
-        <f t="shared" si="1"/>
+      <c r="E17" s="20">
+        <f t="shared" si="0"/>
+        <v>121.63333333333334</v>
+      </c>
+      <c r="F17" s="23">
+        <f t="shared" si="1"/>
+        <v>5.4015020219526158E-2</v>
+      </c>
+      <c r="G17" s="16">
+        <f t="shared" si="3"/>
         <v>0.1101604278074866</v>
       </c>
-      <c r="F17" s="16">
-        <f t="shared" si="2"/>
+      <c r="H17" s="16">
+        <f t="shared" si="4"/>
         <v>-1.5842839036755384E-2</v>
       </c>
-      <c r="G17" s="16">
-        <f t="shared" si="3"/>
+      <c r="I17" s="16">
+        <f t="shared" si="5"/>
         <v>0.1148577449947312</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>27210</v>
       </c>
@@ -1522,20 +1698,28 @@
       <c r="D18" s="14">
         <v>141.69999999999999</v>
       </c>
-      <c r="E18" s="16">
-        <f t="shared" si="1"/>
+      <c r="E18" s="20">
+        <f t="shared" si="0"/>
+        <v>147.03333333333333</v>
+      </c>
+      <c r="F18" s="23">
+        <f t="shared" si="1"/>
+        <v>0.20882433543436549</v>
+      </c>
+      <c r="G18" s="16">
+        <f t="shared" si="3"/>
         <v>6.1657032755298706E-2</v>
       </c>
-      <c r="F18" s="16">
-        <f t="shared" si="2"/>
+      <c r="H18" s="16">
+        <f t="shared" si="4"/>
         <v>0.21828718609143577</v>
       </c>
-      <c r="G18" s="16">
-        <f t="shared" si="3"/>
+      <c r="I18" s="16">
+        <f t="shared" si="5"/>
         <v>0.3393194706994328</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>27575</v>
       </c>
@@ -1548,20 +1732,28 @@
       <c r="D19" s="13">
         <v>177.2</v>
       </c>
-      <c r="E19" s="16">
-        <f t="shared" si="1"/>
+      <c r="E19" s="20">
+        <f t="shared" si="0"/>
+        <v>192.6</v>
+      </c>
+      <c r="F19" s="23">
+        <f t="shared" si="1"/>
+        <v>0.30990705055542961</v>
+      </c>
+      <c r="G19" s="16">
+        <f t="shared" si="3"/>
         <v>0.25771324863883838</v>
       </c>
-      <c r="F19" s="16">
-        <f t="shared" si="2"/>
+      <c r="H19" s="16">
+        <f t="shared" si="4"/>
         <v>0.38477801268498951</v>
       </c>
-      <c r="G19" s="16">
-        <f t="shared" si="3"/>
+      <c r="I19" s="16">
+        <f t="shared" si="5"/>
         <v>0.25052928722653495</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>27941</v>
       </c>
@@ -1574,20 +1766,28 @@
       <c r="D20" s="14">
         <v>190.3</v>
       </c>
-      <c r="E20" s="16">
-        <f t="shared" si="1"/>
+      <c r="E20" s="20">
+        <f t="shared" si="0"/>
+        <v>203.93333333333331</v>
+      </c>
+      <c r="F20" s="23">
+        <f t="shared" si="1"/>
+        <v>5.8843890619591457E-2</v>
+      </c>
+      <c r="G20" s="16">
+        <f t="shared" si="3"/>
         <v>9.0187590187590191E-2</v>
       </c>
-      <c r="F20" s="16">
-        <f t="shared" si="2"/>
+      <c r="H20" s="16">
+        <f t="shared" si="4"/>
         <v>3.2061068702289988E-2</v>
       </c>
-      <c r="G20" s="16">
-        <f t="shared" si="3"/>
+      <c r="I20" s="16">
+        <f t="shared" si="5"/>
         <v>7.3927765237020451E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>28306</v>
       </c>
@@ -1600,20 +1800,28 @@
       <c r="D21" s="13">
         <v>230.2</v>
       </c>
-      <c r="E21" s="16">
-        <f t="shared" si="1"/>
+      <c r="E21" s="20">
+        <f t="shared" si="0"/>
+        <v>237.9</v>
+      </c>
+      <c r="F21" s="23">
+        <f t="shared" si="1"/>
+        <v>0.16655769859431205</v>
+      </c>
+      <c r="G21" s="16">
+        <f t="shared" si="3"/>
         <v>0.12508272667107881</v>
       </c>
-      <c r="F21" s="16">
-        <f t="shared" si="2"/>
+      <c r="H21" s="16">
+        <f t="shared" si="4"/>
         <v>0.15939349112426046</v>
       </c>
-      <c r="G21" s="16">
-        <f t="shared" si="3"/>
+      <c r="I21" s="16">
+        <f t="shared" si="5"/>
         <v>0.20966894377298989</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>28671</v>
       </c>
@@ -1626,20 +1834,28 @@
       <c r="D22" s="14">
         <v>281.7</v>
       </c>
-      <c r="E22" s="16">
-        <f t="shared" si="1"/>
+      <c r="E22" s="20">
+        <f t="shared" si="0"/>
+        <v>287.9666666666667</v>
+      </c>
+      <c r="F22" s="23">
+        <f t="shared" si="1"/>
+        <v>0.21045257110830892</v>
+      </c>
+      <c r="G22" s="16">
+        <f t="shared" si="3"/>
         <v>0.22352941176470589</v>
       </c>
-      <c r="F22" s="16">
-        <f t="shared" si="2"/>
+      <c r="H22" s="16">
+        <f t="shared" si="4"/>
         <v>0.19362041467304622</v>
       </c>
-      <c r="G22" s="16">
-        <f t="shared" si="3"/>
+      <c r="I22" s="16">
+        <f t="shared" si="5"/>
         <v>0.22371850564726325</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>29036</v>
       </c>
@@ -1652,20 +1868,28 @@
       <c r="D23" s="13">
         <v>339.6</v>
       </c>
-      <c r="E23" s="16">
-        <f t="shared" si="1"/>
+      <c r="E23" s="20">
+        <f t="shared" si="0"/>
+        <v>341.93333333333339</v>
+      </c>
+      <c r="F23" s="23">
+        <f t="shared" si="1"/>
+        <v>0.18740594976270411</v>
+      </c>
+      <c r="G23" s="16">
+        <f t="shared" si="3"/>
         <v>0.16874999999999998</v>
       </c>
-      <c r="F23" s="16">
-        <f t="shared" si="2"/>
+      <c r="H23" s="16">
+        <f t="shared" si="4"/>
         <v>0.18412613575628017</v>
       </c>
-      <c r="G23" s="16">
-        <f t="shared" si="3"/>
+      <c r="I23" s="16">
+        <f t="shared" si="5"/>
         <v>0.20553780617678394</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>29402</v>
       </c>
@@ -1678,20 +1902,28 @@
       <c r="D24" s="14">
         <v>376.5</v>
       </c>
-      <c r="E24" s="16">
-        <f t="shared" si="1"/>
+      <c r="E24" s="20">
+        <f t="shared" si="0"/>
+        <v>395</v>
+      </c>
+      <c r="F24" s="23">
+        <f t="shared" si="1"/>
+        <v>0.15519594462858236</v>
+      </c>
+      <c r="G24" s="16">
+        <f t="shared" si="3"/>
         <v>0.11929247223364882</v>
       </c>
-      <c r="F24" s="16">
-        <f t="shared" si="2"/>
+      <c r="H24" s="16">
+        <f t="shared" si="4"/>
         <v>0.21056194989844268</v>
       </c>
-      <c r="G24" s="16">
-        <f t="shared" si="3"/>
+      <c r="I24" s="16">
+        <f t="shared" si="5"/>
         <v>0.10865724381625434</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>29767</v>
       </c>
@@ -1704,20 +1936,28 @@
       <c r="D25" s="13">
         <v>464</v>
       </c>
-      <c r="E25" s="16">
-        <f t="shared" si="1"/>
+      <c r="E25" s="20">
+        <f t="shared" si="0"/>
+        <v>499.63333333333338</v>
+      </c>
+      <c r="F25" s="23">
+        <f t="shared" si="1"/>
+        <v>0.26489451476793263</v>
+      </c>
+      <c r="G25" s="16">
+        <f t="shared" si="3"/>
         <v>0.23594266813671438</v>
       </c>
-      <c r="F25" s="16">
-        <f t="shared" si="2"/>
+      <c r="H25" s="16">
+        <f t="shared" si="4"/>
         <v>0.30238627889634612</v>
       </c>
-      <c r="G25" s="16">
-        <f t="shared" si="3"/>
+      <c r="I25" s="16">
+        <f t="shared" si="5"/>
         <v>0.23240371845949534</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>30132</v>
       </c>
@@ -1730,20 +1970,28 @@
       <c r="D26" s="14">
         <v>515.4</v>
       </c>
-      <c r="E26" s="16">
-        <f t="shared" si="1"/>
+      <c r="E26" s="20">
+        <f t="shared" si="0"/>
+        <v>575.69999999999993</v>
+      </c>
+      <c r="F26" s="23">
+        <f t="shared" si="1"/>
+        <v>0.15224497965174436</v>
+      </c>
+      <c r="G26" s="16">
+        <f t="shared" si="3"/>
         <v>3.3006244424620773E-2</v>
       </c>
-      <c r="F26" s="16">
-        <f t="shared" si="2"/>
+      <c r="H26" s="16">
+        <f t="shared" si="4"/>
         <v>0.23718866304036634</v>
       </c>
-      <c r="G26" s="16">
-        <f t="shared" si="3"/>
+      <c r="I26" s="16">
+        <f t="shared" si="5"/>
         <v>0.11077586206896547</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>30497</v>
       </c>
@@ -1756,20 +2004,28 @@
       <c r="D27" s="13">
         <v>366.5</v>
       </c>
-      <c r="E27" s="16">
-        <f t="shared" si="1"/>
+      <c r="E27" s="20">
+        <f t="shared" si="0"/>
+        <v>419.4666666666667</v>
+      </c>
+      <c r="F27" s="23">
+        <f t="shared" si="1"/>
+        <v>-0.27137976955590282</v>
+      </c>
+      <c r="G27" s="16">
+        <f t="shared" si="3"/>
         <v>-0.1830742659758203</v>
       </c>
-      <c r="F27" s="16">
-        <f t="shared" si="2"/>
+      <c r="H27" s="16">
+        <f t="shared" si="4"/>
         <v>-0.29642485248177708</v>
       </c>
-      <c r="G27" s="16">
-        <f t="shared" si="3"/>
+      <c r="I27" s="16">
+        <f t="shared" si="5"/>
         <v>-0.28890182382615442</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>30863</v>
       </c>
@@ -1782,20 +2038,28 @@
       <c r="D28" s="14">
         <v>329.2</v>
       </c>
-      <c r="E28" s="16">
-        <f t="shared" si="1"/>
+      <c r="E28" s="20">
+        <f t="shared" si="0"/>
+        <v>360.36666666666673</v>
+      </c>
+      <c r="F28" s="23">
+        <f t="shared" si="1"/>
+        <v>-0.14089319771137943</v>
+      </c>
+      <c r="G28" s="16">
+        <f t="shared" si="3"/>
         <v>-7.646229739252991E-2</v>
       </c>
-      <c r="F28" s="16">
-        <f t="shared" si="2"/>
+      <c r="H28" s="16">
+        <f t="shared" si="4"/>
         <v>-0.19454037164939977</v>
       </c>
-      <c r="G28" s="16">
-        <f t="shared" si="3"/>
+      <c r="I28" s="16">
+        <f t="shared" si="5"/>
         <v>-0.1017735334242838</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>31228</v>
       </c>
@@ -1808,20 +2072,28 @@
       <c r="D29" s="13">
         <v>372.3</v>
       </c>
-      <c r="E29" s="16">
-        <f t="shared" si="1"/>
+      <c r="E29" s="20">
+        <f t="shared" si="0"/>
+        <v>383.79999999999995</v>
+      </c>
+      <c r="F29" s="23">
+        <f t="shared" si="1"/>
+        <v>6.5026362038664007E-2</v>
+      </c>
+      <c r="G29" s="16">
+        <f t="shared" si="3"/>
         <v>3.1667302556276054E-2</v>
       </c>
-      <c r="F29" s="16">
-        <f t="shared" si="2"/>
+      <c r="H29" s="16">
+        <f t="shared" si="4"/>
         <v>3.8587178440179615E-2</v>
       </c>
-      <c r="G29" s="16">
-        <f t="shared" si="3"/>
+      <c r="I29" s="16">
+        <f t="shared" si="5"/>
         <v>0.13092345078979351</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>31593</v>
       </c>
@@ -1834,20 +2106,28 @@
       <c r="D30" s="14">
         <v>389.2</v>
       </c>
-      <c r="E30" s="16">
-        <f t="shared" si="1"/>
+      <c r="E30" s="20">
+        <f t="shared" si="0"/>
+        <v>399</v>
+      </c>
+      <c r="F30" s="23">
+        <f t="shared" si="1"/>
+        <v>3.9603960396039729E-2</v>
+      </c>
+      <c r="G30" s="16">
+        <f>(B30-B29)/B29</f>
         <v>5.3624260355029589E-2</v>
       </c>
-      <c r="F30" s="16">
-        <f t="shared" si="2"/>
+      <c r="H30" s="16">
+        <f t="shared" si="4"/>
         <v>2.7914291330843305E-2</v>
       </c>
-      <c r="G30" s="16">
-        <f t="shared" si="3"/>
+      <c r="I30" s="16">
+        <f t="shared" si="5"/>
         <v>4.5393499865699641E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>31958</v>
       </c>
@@ -1860,20 +2140,28 @@
       <c r="D31" s="13">
         <v>259.10000000000002</v>
       </c>
-      <c r="E31" s="16">
-        <f t="shared" si="1"/>
+      <c r="E31" s="20">
+        <f t="shared" si="0"/>
+        <v>295.16666666666669</v>
+      </c>
+      <c r="F31" s="23">
+        <f t="shared" si="1"/>
+        <v>-0.26023391812865493</v>
+      </c>
+      <c r="G31" s="16">
+        <f>(B31-B30)/B30</f>
         <v>-0.13653913653913646</v>
       </c>
-      <c r="F31" s="16">
-        <f t="shared" si="2"/>
+      <c r="H31" s="16">
+        <f t="shared" si="4"/>
         <v>-0.27251864601262193</v>
       </c>
-      <c r="G31" s="16">
-        <f t="shared" si="3"/>
+      <c r="I31" s="16">
+        <f t="shared" si="5"/>
         <v>-0.33427543679342231</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>32324</v>
       </c>
@@ -1886,20 +2174,28 @@
       <c r="D32" s="14">
         <v>366.4</v>
       </c>
-      <c r="E32" s="16">
-        <f t="shared" si="1"/>
+      <c r="E32" s="20">
+        <f t="shared" si="0"/>
+        <v>368.7</v>
+      </c>
+      <c r="F32" s="23">
+        <f t="shared" si="1"/>
+        <v>0.24912478825522291</v>
+      </c>
+      <c r="G32" s="16">
+        <f t="shared" si="3"/>
         <v>0.13577235772357715</v>
       </c>
-      <c r="F32" s="16">
-        <f t="shared" si="2"/>
+      <c r="H32" s="16">
+        <f t="shared" si="4"/>
         <v>0.21004206098843334</v>
       </c>
-      <c r="G32" s="16">
-        <f t="shared" si="3"/>
+      <c r="I32" s="16">
+        <f t="shared" si="5"/>
         <v>0.41412582014666133</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>32689</v>
       </c>
@@ -1912,20 +2208,28 @@
       <c r="D33" s="13">
         <v>355.4</v>
       </c>
-      <c r="E33" s="16">
-        <f t="shared" si="1"/>
+      <c r="E33" s="20">
+        <f t="shared" si="0"/>
+        <v>365.16666666666669</v>
+      </c>
+      <c r="F33" s="23">
+        <f t="shared" si="1"/>
+        <v>-9.5832203236596233E-3</v>
+      </c>
+      <c r="G33" s="16">
+        <f t="shared" si="3"/>
         <v>1.037938439513255E-2</v>
       </c>
-      <c r="F33" s="16">
-        <f t="shared" si="2"/>
+      <c r="H33" s="16">
+        <f t="shared" si="4"/>
         <v>-5.4312404953291331E-3</v>
       </c>
-      <c r="G33" s="16">
-        <f t="shared" si="3"/>
+      <c r="I33" s="16">
+        <f t="shared" si="5"/>
         <v>-3.0021834061135372E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>33054</v>
       </c>
@@ -1938,20 +2242,28 @@
       <c r="D34" s="14">
         <v>367.5</v>
       </c>
-      <c r="E34" s="16">
-        <f t="shared" si="1"/>
+      <c r="E34" s="20">
+        <f t="shared" si="0"/>
+        <v>386.86666666666662</v>
+      </c>
+      <c r="F34" s="23">
+        <f t="shared" si="1"/>
+        <v>5.9424920127795336E-2</v>
+      </c>
+      <c r="G34" s="16">
+        <f t="shared" si="3"/>
         <v>0.13992206872121857</v>
       </c>
-      <c r="F34" s="16">
-        <f t="shared" si="2"/>
+      <c r="H34" s="16">
+        <f t="shared" si="4"/>
         <v>2.9488859764089121E-2</v>
       </c>
-      <c r="G34" s="16">
-        <f t="shared" si="3"/>
+      <c r="I34" s="16">
+        <f t="shared" si="5"/>
         <v>3.4046145188520047E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>33419</v>
       </c>
@@ -1964,20 +2276,28 @@
       <c r="D35" s="13">
         <v>441.2</v>
       </c>
-      <c r="E35" s="16">
-        <f t="shared" si="1"/>
+      <c r="E35" s="20">
+        <f>SUM(B35:D35)/3</f>
+        <v>431.56666666666666</v>
+      </c>
+      <c r="F35" s="23">
+        <f t="shared" si="1"/>
+        <v>0.11554368430122364</v>
+      </c>
+      <c r="G35" s="16">
+        <f t="shared" si="3"/>
         <v>7.799875699192034E-2</v>
       </c>
-      <c r="F35" s="16">
-        <f t="shared" si="2"/>
+      <c r="H35" s="16">
+        <f t="shared" si="4"/>
         <v>7.4899214937407199E-2</v>
       </c>
-      <c r="G35" s="16">
-        <f t="shared" si="3"/>
+      <c r="I35" s="16">
+        <f t="shared" si="5"/>
         <v>0.20054421768707481</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>33785</v>
       </c>
@@ -1990,20 +2310,28 @@
       <c r="D36" s="14">
         <v>357.6</v>
       </c>
-      <c r="E36" s="16">
-        <f t="shared" si="1"/>
+      <c r="E36" s="20">
+        <f t="shared" ref="E36:E49" si="6">SUM(B36:D36)/3</f>
+        <v>382</v>
+      </c>
+      <c r="F36" s="23">
+        <f>(E36-E35)/E35</f>
+        <v>-0.11485286166679538</v>
+      </c>
+      <c r="G36" s="16">
+        <f t="shared" si="3"/>
         <v>4.4393196886710971E-2</v>
       </c>
-      <c r="F36" s="16">
-        <f t="shared" si="2"/>
+      <c r="H36" s="16">
+        <f t="shared" si="4"/>
         <v>-0.15890248716936439</v>
       </c>
-      <c r="G36" s="16">
-        <f t="shared" si="3"/>
+      <c r="I36" s="16">
+        <f t="shared" si="5"/>
         <v>-0.18948322756119668</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>34150</v>
       </c>
@@ -2016,20 +2344,28 @@
       <c r="D37" s="13">
         <v>387.7</v>
       </c>
-      <c r="E37" s="16">
-        <f t="shared" si="1"/>
+      <c r="E37" s="20">
+        <f t="shared" si="6"/>
+        <v>421.83333333333331</v>
+      </c>
+      <c r="F37" s="23">
+        <f t="shared" ref="F37:F51" si="7">(E37-E36)/E36</f>
+        <v>0.10427574171029663</v>
+      </c>
+      <c r="G37" s="16">
+        <f t="shared" si="3"/>
         <v>-1.5732818106541507E-2</v>
       </c>
-      <c r="F37" s="16">
-        <f t="shared" si="2"/>
+      <c r="H37" s="16">
+        <f t="shared" si="4"/>
         <v>0.22318704529453184</v>
       </c>
-      <c r="G37" s="16">
-        <f t="shared" si="3"/>
+      <c r="I37" s="16">
+        <f t="shared" si="5"/>
         <v>8.4172259507829875E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>34515</v>
       </c>
@@ -2042,20 +2378,28 @@
       <c r="D38" s="14">
         <v>491.5</v>
       </c>
-      <c r="E38" s="16">
-        <f t="shared" si="1"/>
+      <c r="E38" s="20">
+        <f t="shared" si="6"/>
+        <v>478.7</v>
+      </c>
+      <c r="F38" s="23">
+        <f t="shared" si="7"/>
+        <v>0.13480837613591468</v>
+      </c>
+      <c r="G38" s="16">
+        <f t="shared" si="3"/>
         <v>0.14834548513740878</v>
       </c>
-      <c r="F38" s="16">
-        <f t="shared" si="2"/>
+      <c r="H38" s="16">
+        <f t="shared" si="4"/>
         <v>2.6669224865694504E-2</v>
       </c>
-      <c r="G38" s="16">
-        <f t="shared" si="3"/>
+      <c r="I38" s="16">
+        <f t="shared" si="5"/>
         <v>0.26773278307970083</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
         <v>34880</v>
       </c>
@@ -2068,20 +2412,28 @@
       <c r="D39" s="13">
         <v>481.2</v>
       </c>
-      <c r="E39" s="16">
-        <f t="shared" si="1"/>
+      <c r="E39" s="20">
+        <f t="shared" si="6"/>
+        <v>508.90000000000003</v>
+      </c>
+      <c r="F39" s="23">
+        <f t="shared" si="7"/>
+        <v>6.3087528723626579E-2</v>
+      </c>
+      <c r="G39" s="16">
+        <f t="shared" si="3"/>
         <v>1.5384615384615413E-2</v>
       </c>
-      <c r="F39" s="16">
-        <f t="shared" si="2"/>
+      <c r="H39" s="16">
+        <f t="shared" si="4"/>
         <v>0.17678938516165207</v>
       </c>
-      <c r="G39" s="16">
-        <f t="shared" si="3"/>
+      <c r="I39" s="16">
+        <f t="shared" si="5"/>
         <v>-2.0956256358087511E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>35246</v>
       </c>
@@ -2094,20 +2446,28 @@
       <c r="D40" s="14">
         <v>541</v>
       </c>
-      <c r="E40" s="16">
-        <f t="shared" si="1"/>
+      <c r="E40" s="20">
+        <f t="shared" si="6"/>
+        <v>499.33333333333331</v>
+      </c>
+      <c r="F40" s="23">
+        <f t="shared" si="7"/>
+        <v>-1.8798716185236233E-2</v>
+      </c>
+      <c r="G40" s="16">
+        <f t="shared" si="3"/>
         <v>-0.17989417989417991</v>
       </c>
-      <c r="F40" s="16">
-        <f t="shared" si="2"/>
+      <c r="H40" s="16">
+        <f t="shared" si="4"/>
         <v>-2.175639193266642E-2</v>
       </c>
-      <c r="G40" s="16">
-        <f t="shared" si="3"/>
+      <c r="I40" s="16">
+        <f t="shared" si="5"/>
         <v>0.12427265170407317</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="12">
         <v>35611</v>
       </c>
@@ -2120,20 +2480,28 @@
       <c r="D41" s="13">
         <v>655.6</v>
       </c>
-      <c r="E41" s="16">
-        <f t="shared" si="1"/>
+      <c r="E41" s="20">
+        <f t="shared" si="6"/>
+        <v>609.93333333333339</v>
+      </c>
+      <c r="F41" s="23">
+        <f t="shared" si="7"/>
+        <v>0.2214953271028039</v>
+      </c>
+      <c r="G41" s="16">
+        <f t="shared" si="3"/>
         <v>0.30674486803519069</v>
       </c>
-      <c r="F41" s="16">
-        <f t="shared" si="2"/>
+      <c r="H41" s="16">
+        <f t="shared" si="4"/>
         <v>0.18279220779220784</v>
       </c>
-      <c r="G41" s="16">
-        <f t="shared" si="3"/>
+      <c r="I41" s="16">
+        <f t="shared" si="5"/>
         <v>0.21182994454713497</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>35976</v>
       </c>
@@ -2146,20 +2514,28 @@
       <c r="D42" s="14">
         <v>973.2</v>
       </c>
-      <c r="E42" s="16">
-        <f t="shared" si="1"/>
+      <c r="E42" s="20">
+        <f t="shared" si="6"/>
+        <v>784.93333333333339</v>
+      </c>
+      <c r="F42" s="23">
+        <f t="shared" si="7"/>
+        <v>0.28691660290742155</v>
+      </c>
+      <c r="G42" s="16">
+        <f t="shared" si="3"/>
         <v>0.27019748653500891</v>
       </c>
-      <c r="F42" s="16">
-        <f t="shared" si="2"/>
+      <c r="H42" s="16">
+        <f t="shared" si="4"/>
         <v>0.11940708207521274</v>
       </c>
-      <c r="G42" s="16">
-        <f t="shared" si="3"/>
+      <c r="I42" s="16">
+        <f t="shared" si="5"/>
         <v>0.48444173276388042</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>36341</v>
       </c>
@@ -2172,20 +2548,28 @@
       <c r="D43" s="13">
         <v>1115.5</v>
       </c>
-      <c r="E43" s="16">
-        <f t="shared" si="1"/>
+      <c r="E43" s="20">
+        <f t="shared" si="6"/>
+        <v>898.9666666666667</v>
+      </c>
+      <c r="F43" s="23">
+        <f t="shared" si="7"/>
+        <v>0.14527773059283161</v>
+      </c>
+      <c r="G43" s="16">
+        <f t="shared" si="3"/>
         <v>0.3833922261484099</v>
       </c>
-      <c r="F43" s="16">
-        <f t="shared" si="2"/>
+      <c r="H43" s="16">
+        <f t="shared" si="4"/>
         <v>-2.1088769004413983E-2</v>
       </c>
-      <c r="G43" s="16">
-        <f t="shared" si="3"/>
+      <c r="I43" s="16">
+        <f t="shared" si="5"/>
         <v>0.14621866009042328</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="12">
         <v>36707</v>
       </c>
@@ -2198,20 +2582,28 @@
       <c r="D44" s="14">
         <v>1075.4000000000001</v>
       </c>
-      <c r="E44" s="16">
-        <f t="shared" si="1"/>
+      <c r="E44" s="20">
+        <f t="shared" si="6"/>
+        <v>808.56666666666661</v>
+      </c>
+      <c r="F44" s="23">
+        <f t="shared" si="7"/>
+        <v>-0.1005599021098299</v>
+      </c>
+      <c r="G44" s="16">
+        <f t="shared" si="3"/>
         <v>-0.24214559386973183</v>
       </c>
-      <c r="F44" s="16">
-        <f t="shared" si="2"/>
+      <c r="H44" s="16">
+        <f t="shared" si="4"/>
         <v>-5.1978957915831667E-2</v>
       </c>
-      <c r="G44" s="16">
-        <f t="shared" si="3"/>
+      <c r="I44" s="16">
+        <f t="shared" si="5"/>
         <v>-3.5948005378753839E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="12">
         <v>37072</v>
       </c>
@@ -2224,20 +2616,28 @@
       <c r="D45" s="13">
         <v>1620.4</v>
       </c>
-      <c r="E45" s="16">
-        <f t="shared" si="1"/>
+      <c r="E45" s="20">
+        <f t="shared" si="6"/>
+        <v>1082</v>
+      </c>
+      <c r="F45" s="23">
+        <f t="shared" si="7"/>
+        <v>0.33817042503194966</v>
+      </c>
+      <c r="G45" s="16">
+        <f t="shared" si="3"/>
         <v>0.22868217054263573</v>
       </c>
-      <c r="F45" s="16">
-        <f t="shared" si="2"/>
+      <c r="H45" s="16">
+        <f t="shared" si="4"/>
         <v>0.1844365173734972</v>
       </c>
-      <c r="G45" s="16">
-        <f t="shared" si="3"/>
+      <c r="I45" s="16">
+        <f t="shared" si="5"/>
         <v>0.50678817184303515</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="12">
         <v>37437</v>
       </c>
@@ -2250,20 +2650,28 @@
       <c r="D46" s="14">
         <v>1673.4</v>
       </c>
-      <c r="E46" s="16">
-        <f t="shared" si="1"/>
+      <c r="E46" s="20">
+        <f t="shared" si="6"/>
+        <v>1182.7</v>
+      </c>
+      <c r="F46" s="23">
+        <f t="shared" si="7"/>
+        <v>9.3068391866913167E-2</v>
+      </c>
+      <c r="G46" s="16">
+        <f t="shared" si="3"/>
         <v>0.21080784528871202</v>
       </c>
-      <c r="F46" s="16">
-        <f t="shared" si="2"/>
+      <c r="H46" s="16">
+        <f t="shared" si="4"/>
         <v>0.10641383156720577</v>
       </c>
-      <c r="G46" s="16">
-        <f t="shared" si="3"/>
+      <c r="I46" s="16">
+        <f t="shared" si="5"/>
         <v>3.2707973339916069E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>37802</v>
       </c>
@@ -2276,20 +2684,28 @@
       <c r="D47" s="13">
         <v>2065.1</v>
       </c>
-      <c r="E47" s="16">
-        <f t="shared" si="1"/>
+      <c r="E47" s="20">
+        <f t="shared" si="6"/>
+        <v>1402.8</v>
+      </c>
+      <c r="F47" s="23">
+        <f t="shared" si="7"/>
+        <v>0.18609960260421063</v>
+      </c>
+      <c r="G47" s="16">
+        <f t="shared" si="3"/>
         <v>0.17501132759401905</v>
       </c>
-      <c r="F47" s="16">
-        <f t="shared" si="2"/>
+      <c r="H47" s="16">
+        <f t="shared" si="4"/>
         <v>0.11503175723359212</v>
       </c>
-      <c r="G47" s="16">
-        <f t="shared" si="3"/>
+      <c r="I47" s="16">
+        <f t="shared" si="5"/>
         <v>0.23407433966774219</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="12">
         <v>38168</v>
       </c>
@@ -2302,20 +2718,28 @@
       <c r="D48" s="14">
         <v>1977.3</v>
       </c>
-      <c r="E48" s="16">
-        <f t="shared" si="1"/>
+      <c r="E48" s="20">
+        <f t="shared" si="6"/>
+        <v>1711.8333333333333</v>
+      </c>
+      <c r="F48" s="23">
+        <f t="shared" si="7"/>
+        <v>0.22029750023761999</v>
+      </c>
+      <c r="G48" s="16">
+        <f t="shared" si="3"/>
         <v>0.38995469006073463</v>
       </c>
-      <c r="F48" s="16">
-        <f t="shared" si="2"/>
+      <c r="H48" s="16">
+        <f t="shared" si="4"/>
         <v>0.55189873417721524</v>
       </c>
-      <c r="G48" s="16">
-        <f t="shared" si="3"/>
+      <c r="I48" s="16">
+        <f t="shared" si="5"/>
         <v>-4.2516100915209895E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="12">
         <v>38533</v>
       </c>
@@ -2328,20 +2752,28 @@
       <c r="D49" s="13">
         <v>2392.9</v>
       </c>
-      <c r="E49" s="16">
-        <f t="shared" si="1"/>
+      <c r="E49" s="20">
+        <f t="shared" si="6"/>
+        <v>1936.9666666666665</v>
+      </c>
+      <c r="F49" s="23">
+        <f t="shared" si="7"/>
+        <v>0.13151591860578321</v>
+      </c>
+      <c r="G49" s="16">
+        <f t="shared" si="3"/>
         <v>0.33194617838812607</v>
       </c>
-      <c r="F49" s="16">
-        <f t="shared" si="2"/>
+      <c r="H49" s="16">
+        <f t="shared" si="4"/>
         <v>-0.12747611279422055</v>
       </c>
-      <c r="G49" s="16">
-        <f t="shared" si="3"/>
+      <c r="I49" s="16">
+        <f t="shared" si="5"/>
         <v>0.21018560663531086</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="12">
         <v>38898</v>
       </c>
@@ -2354,20 +2786,28 @@
       <c r="D50" s="14">
         <v>2664.6</v>
       </c>
-      <c r="E50" s="16">
-        <f t="shared" si="1"/>
+      <c r="E50" s="20">
+        <f>SUM(B50:D50)/3</f>
+        <v>2279.7999999999997</v>
+      </c>
+      <c r="F50" s="23">
+        <f t="shared" si="7"/>
+        <v>0.17699495775181123</v>
+      </c>
+      <c r="G50" s="16">
+        <f t="shared" si="3"/>
         <v>0.16569464694855229</v>
       </c>
-      <c r="F50" s="16">
-        <f t="shared" si="2"/>
+      <c r="H50" s="16">
+        <f t="shared" si="4"/>
         <v>0.29286858974358987</v>
       </c>
-      <c r="G50" s="16">
-        <f t="shared" si="3"/>
+      <c r="I50" s="16">
+        <f t="shared" si="5"/>
         <v>0.11354423502862628</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="12">
         <v>39263</v>
       </c>
@@ -2380,26 +2820,35 @@
       <c r="D51" s="13">
         <v>6131.2</v>
       </c>
-      <c r="E51" s="16">
-        <f t="shared" si="1"/>
+      <c r="E51" s="20">
+        <f>SUM(B51:D51)/3</f>
+        <v>4679.5</v>
+      </c>
+      <c r="F51" s="23">
+        <f t="shared" si="7"/>
+        <v>1.05259233266076</v>
+      </c>
+      <c r="G51" s="16">
+        <f t="shared" si="3"/>
         <v>0.78700973822925058</v>
       </c>
-      <c r="F51" s="16">
-        <f t="shared" si="2"/>
+      <c r="H51" s="16">
+        <f t="shared" si="4"/>
         <v>1.0178184071893399</v>
       </c>
-      <c r="G51" s="16">
-        <f t="shared" si="3"/>
+      <c r="I51" s="16">
+        <f t="shared" si="5"/>
         <v>1.3009832620280717</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Small change to data
</commit_message>
<xml_diff>
--- a/Simulation & Risk/Data/Analysis_Data.xlsx
+++ b/Simulation & Risk/Data/Analysis_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Desktop\IAA\Spring 1\spring1-orange5\Simulation &amp; Risk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9C3C89-22BF-4998-AC44-FDCF3A7D2DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3BDC41-5FF6-48A0-A6B7-86B67A54A248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>High Oil Price</t>
   </si>
@@ -307,18 +307,18 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -663,7 +663,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -675,10 +675,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1155,7 +1155,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,16 +1175,16 @@
       <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -1202,7 +1202,7 @@
       <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1228,11 +1228,13 @@
       <c r="D4" s="11">
         <v>44</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="18">
         <f t="shared" ref="E4:E34" si="0">SUM(B4:D4)/3</f>
         <v>66.3</v>
       </c>
-      <c r="F4" s="22"/>
+      <c r="F4" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="G4" t="s">
         <v>13</v>
       </c>
@@ -1256,11 +1258,11 @@
       <c r="D5" s="13">
         <v>45.2</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="18">
         <f t="shared" si="0"/>
         <v>63.733333333333327</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="21">
         <f t="shared" ref="F5:F35" si="1">(E5-E4)/E4</f>
         <v>-3.8712921065862292E-2</v>
       </c>
@@ -1290,11 +1292,11 @@
       <c r="D6" s="14">
         <v>50.8</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <f t="shared" si="0"/>
         <v>67.366666666666674</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="21">
         <f t="shared" si="1"/>
         <v>5.7008368200837038E-2</v>
       </c>
@@ -1324,11 +1326,11 @@
       <c r="D7" s="13">
         <v>48.2</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="18">
         <f t="shared" si="0"/>
         <v>64.133333333333326</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="21">
         <f t="shared" si="1"/>
         <v>-4.7996041563582607E-2</v>
       </c>
@@ -1358,11 +1360,11 @@
       <c r="D8" s="14">
         <v>48.5</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="18">
         <f t="shared" si="0"/>
         <v>67.966666666666669</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="21">
         <f t="shared" si="1"/>
         <v>5.9771309771309927E-2</v>
       </c>
@@ -1392,11 +1394,11 @@
       <c r="D9" s="13">
         <v>53.1</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="18">
         <f t="shared" si="0"/>
         <v>70.533333333333331</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="21">
         <f t="shared" si="1"/>
         <v>3.7763609612555114E-2</v>
       </c>
@@ -1426,11 +1428,11 @@
       <c r="D10" s="14">
         <v>56.9</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="18">
         <f t="shared" si="0"/>
         <v>84.3</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="21">
         <f t="shared" si="1"/>
         <v>0.19517958412098299</v>
       </c>
@@ -1460,11 +1462,11 @@
       <c r="D11" s="13">
         <v>61.5</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="18">
         <f t="shared" si="0"/>
         <v>89.7</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="21">
         <f t="shared" si="1"/>
         <v>6.4056939501779431E-2</v>
       </c>
@@ -1494,11 +1496,11 @@
       <c r="D12" s="14">
         <v>66.2</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="18">
         <f t="shared" si="0"/>
         <v>97.933333333333337</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="21">
         <f t="shared" si="1"/>
         <v>9.1787439613526575E-2</v>
       </c>
@@ -1528,11 +1530,11 @@
       <c r="D13" s="13">
         <v>70.2</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="18">
         <f t="shared" si="0"/>
         <v>103.66666666666667</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="21">
         <f t="shared" si="1"/>
         <v>5.8543226684819615E-2</v>
       </c>
@@ -1562,11 +1564,11 @@
       <c r="D14" s="14">
         <v>80.900000000000006</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="18">
         <f t="shared" si="0"/>
         <v>109.43333333333332</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="21">
         <f t="shared" si="1"/>
         <v>5.56270096463021E-2</v>
       </c>
@@ -1596,11 +1598,11 @@
       <c r="D15" s="13">
         <v>86.8</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="18">
         <f t="shared" si="0"/>
         <v>110.60000000000001</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="21">
         <f t="shared" si="1"/>
         <v>1.0660980810234717E-2</v>
       </c>
@@ -1630,11 +1632,11 @@
       <c r="D16" s="14">
         <v>94.9</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="18">
         <f t="shared" si="0"/>
         <v>115.40000000000002</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="21">
         <f t="shared" si="1"/>
         <v>4.3399638336347295E-2</v>
       </c>
@@ -1664,11 +1666,11 @@
       <c r="D17" s="13">
         <v>105.8</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="18">
         <f t="shared" si="0"/>
         <v>121.63333333333334</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="21">
         <f t="shared" si="1"/>
         <v>5.4015020219526158E-2</v>
       </c>
@@ -1698,11 +1700,11 @@
       <c r="D18" s="14">
         <v>141.69999999999999</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="18">
         <f t="shared" si="0"/>
         <v>147.03333333333333</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="21">
         <f t="shared" si="1"/>
         <v>0.20882433543436549</v>
       </c>
@@ -1732,11 +1734,11 @@
       <c r="D19" s="13">
         <v>177.2</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="18">
         <f t="shared" si="0"/>
         <v>192.6</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="21">
         <f t="shared" si="1"/>
         <v>0.30990705055542961</v>
       </c>
@@ -1766,11 +1768,11 @@
       <c r="D20" s="14">
         <v>190.3</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="18">
         <f t="shared" si="0"/>
         <v>203.93333333333331</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="21">
         <f t="shared" si="1"/>
         <v>5.8843890619591457E-2</v>
       </c>
@@ -1800,11 +1802,11 @@
       <c r="D21" s="13">
         <v>230.2</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="18">
         <f t="shared" si="0"/>
         <v>237.9</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="21">
         <f t="shared" si="1"/>
         <v>0.16655769859431205</v>
       </c>
@@ -1834,11 +1836,11 @@
       <c r="D22" s="14">
         <v>281.7</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="18">
         <f t="shared" si="0"/>
         <v>287.9666666666667</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="21">
         <f t="shared" si="1"/>
         <v>0.21045257110830892</v>
       </c>
@@ -1868,11 +1870,11 @@
       <c r="D23" s="13">
         <v>339.6</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="18">
         <f t="shared" si="0"/>
         <v>341.93333333333339</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="21">
         <f t="shared" si="1"/>
         <v>0.18740594976270411</v>
       </c>
@@ -1902,11 +1904,11 @@
       <c r="D24" s="14">
         <v>376.5</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="18">
         <f t="shared" si="0"/>
         <v>395</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="21">
         <f t="shared" si="1"/>
         <v>0.15519594462858236</v>
       </c>
@@ -1936,11 +1938,11 @@
       <c r="D25" s="13">
         <v>464</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="18">
         <f t="shared" si="0"/>
         <v>499.63333333333338</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="21">
         <f t="shared" si="1"/>
         <v>0.26489451476793263</v>
       </c>
@@ -1970,11 +1972,11 @@
       <c r="D26" s="14">
         <v>515.4</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="18">
         <f t="shared" si="0"/>
         <v>575.69999999999993</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="21">
         <f t="shared" si="1"/>
         <v>0.15224497965174436</v>
       </c>
@@ -2004,11 +2006,11 @@
       <c r="D27" s="13">
         <v>366.5</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="18">
         <f t="shared" si="0"/>
         <v>419.4666666666667</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="21">
         <f t="shared" si="1"/>
         <v>-0.27137976955590282</v>
       </c>
@@ -2038,11 +2040,11 @@
       <c r="D28" s="14">
         <v>329.2</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="18">
         <f t="shared" si="0"/>
         <v>360.36666666666673</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="21">
         <f t="shared" si="1"/>
         <v>-0.14089319771137943</v>
       </c>
@@ -2072,11 +2074,11 @@
       <c r="D29" s="13">
         <v>372.3</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="18">
         <f t="shared" si="0"/>
         <v>383.79999999999995</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="21">
         <f t="shared" si="1"/>
         <v>6.5026362038664007E-2</v>
       </c>
@@ -2106,11 +2108,11 @@
       <c r="D30" s="14">
         <v>389.2</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="18">
         <f t="shared" si="0"/>
         <v>399</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="21">
         <f t="shared" si="1"/>
         <v>3.9603960396039729E-2</v>
       </c>
@@ -2140,11 +2142,11 @@
       <c r="D31" s="13">
         <v>259.10000000000002</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="18">
         <f t="shared" si="0"/>
         <v>295.16666666666669</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="21">
         <f t="shared" si="1"/>
         <v>-0.26023391812865493</v>
       </c>
@@ -2174,11 +2176,11 @@
       <c r="D32" s="14">
         <v>366.4</v>
       </c>
-      <c r="E32" s="20">
+      <c r="E32" s="18">
         <f t="shared" si="0"/>
         <v>368.7</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="21">
         <f t="shared" si="1"/>
         <v>0.24912478825522291</v>
       </c>
@@ -2208,11 +2210,11 @@
       <c r="D33" s="13">
         <v>355.4</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E33" s="18">
         <f t="shared" si="0"/>
         <v>365.16666666666669</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="21">
         <f t="shared" si="1"/>
         <v>-9.5832203236596233E-3</v>
       </c>
@@ -2242,11 +2244,11 @@
       <c r="D34" s="14">
         <v>367.5</v>
       </c>
-      <c r="E34" s="20">
+      <c r="E34" s="18">
         <f t="shared" si="0"/>
         <v>386.86666666666662</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="21">
         <f t="shared" si="1"/>
         <v>5.9424920127795336E-2</v>
       </c>
@@ -2276,11 +2278,11 @@
       <c r="D35" s="13">
         <v>441.2</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="18">
         <f>SUM(B35:D35)/3</f>
         <v>431.56666666666666</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="21">
         <f t="shared" si="1"/>
         <v>0.11554368430122364</v>
       </c>
@@ -2310,11 +2312,11 @@
       <c r="D36" s="14">
         <v>357.6</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="18">
         <f t="shared" ref="E36:E49" si="6">SUM(B36:D36)/3</f>
         <v>382</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="21">
         <f>(E36-E35)/E35</f>
         <v>-0.11485286166679538</v>
       </c>
@@ -2344,11 +2346,11 @@
       <c r="D37" s="13">
         <v>387.7</v>
       </c>
-      <c r="E37" s="20">
+      <c r="E37" s="18">
         <f t="shared" si="6"/>
         <v>421.83333333333331</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="21">
         <f t="shared" ref="F37:F51" si="7">(E37-E36)/E36</f>
         <v>0.10427574171029663</v>
       </c>
@@ -2378,11 +2380,11 @@
       <c r="D38" s="14">
         <v>491.5</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="18">
         <f t="shared" si="6"/>
         <v>478.7</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="21">
         <f t="shared" si="7"/>
         <v>0.13480837613591468</v>
       </c>
@@ -2412,11 +2414,11 @@
       <c r="D39" s="13">
         <v>481.2</v>
       </c>
-      <c r="E39" s="20">
+      <c r="E39" s="18">
         <f t="shared" si="6"/>
         <v>508.90000000000003</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="21">
         <f t="shared" si="7"/>
         <v>6.3087528723626579E-2</v>
       </c>
@@ -2446,11 +2448,11 @@
       <c r="D40" s="14">
         <v>541</v>
       </c>
-      <c r="E40" s="20">
+      <c r="E40" s="18">
         <f t="shared" si="6"/>
         <v>499.33333333333331</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="21">
         <f t="shared" si="7"/>
         <v>-1.8798716185236233E-2</v>
       </c>
@@ -2480,11 +2482,11 @@
       <c r="D41" s="13">
         <v>655.6</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="18">
         <f t="shared" si="6"/>
         <v>609.93333333333339</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="21">
         <f t="shared" si="7"/>
         <v>0.2214953271028039</v>
       </c>
@@ -2514,11 +2516,11 @@
       <c r="D42" s="14">
         <v>973.2</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="18">
         <f t="shared" si="6"/>
         <v>784.93333333333339</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="21">
         <f t="shared" si="7"/>
         <v>0.28691660290742155</v>
       </c>
@@ -2548,11 +2550,11 @@
       <c r="D43" s="13">
         <v>1115.5</v>
       </c>
-      <c r="E43" s="20">
+      <c r="E43" s="18">
         <f t="shared" si="6"/>
         <v>898.9666666666667</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="21">
         <f t="shared" si="7"/>
         <v>0.14527773059283161</v>
       </c>
@@ -2582,11 +2584,11 @@
       <c r="D44" s="14">
         <v>1075.4000000000001</v>
       </c>
-      <c r="E44" s="20">
+      <c r="E44" s="18">
         <f t="shared" si="6"/>
         <v>808.56666666666661</v>
       </c>
-      <c r="F44" s="23">
+      <c r="F44" s="21">
         <f t="shared" si="7"/>
         <v>-0.1005599021098299</v>
       </c>
@@ -2616,11 +2618,11 @@
       <c r="D45" s="13">
         <v>1620.4</v>
       </c>
-      <c r="E45" s="20">
+      <c r="E45" s="18">
         <f t="shared" si="6"/>
         <v>1082</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F45" s="21">
         <f t="shared" si="7"/>
         <v>0.33817042503194966</v>
       </c>
@@ -2650,11 +2652,11 @@
       <c r="D46" s="14">
         <v>1673.4</v>
       </c>
-      <c r="E46" s="20">
+      <c r="E46" s="18">
         <f t="shared" si="6"/>
         <v>1182.7</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="21">
         <f t="shared" si="7"/>
         <v>9.3068391866913167E-2</v>
       </c>
@@ -2684,11 +2686,11 @@
       <c r="D47" s="13">
         <v>2065.1</v>
       </c>
-      <c r="E47" s="20">
+      <c r="E47" s="18">
         <f t="shared" si="6"/>
         <v>1402.8</v>
       </c>
-      <c r="F47" s="23">
+      <c r="F47" s="21">
         <f t="shared" si="7"/>
         <v>0.18609960260421063</v>
       </c>
@@ -2718,11 +2720,11 @@
       <c r="D48" s="14">
         <v>1977.3</v>
       </c>
-      <c r="E48" s="20">
+      <c r="E48" s="18">
         <f t="shared" si="6"/>
         <v>1711.8333333333333</v>
       </c>
-      <c r="F48" s="23">
+      <c r="F48" s="21">
         <f t="shared" si="7"/>
         <v>0.22029750023761999</v>
       </c>
@@ -2752,11 +2754,11 @@
       <c r="D49" s="13">
         <v>2392.9</v>
       </c>
-      <c r="E49" s="20">
+      <c r="E49" s="18">
         <f t="shared" si="6"/>
         <v>1936.9666666666665</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F49" s="21">
         <f t="shared" si="7"/>
         <v>0.13151591860578321</v>
       </c>
@@ -2786,11 +2788,11 @@
       <c r="D50" s="14">
         <v>2664.6</v>
       </c>
-      <c r="E50" s="20">
+      <c r="E50" s="18">
         <f>SUM(B50:D50)/3</f>
         <v>2279.7999999999997</v>
       </c>
-      <c r="F50" s="23">
+      <c r="F50" s="21">
         <f t="shared" si="7"/>
         <v>0.17699495775181123</v>
       </c>
@@ -2820,11 +2822,11 @@
       <c r="D51" s="13">
         <v>6131.2</v>
       </c>
-      <c r="E51" s="20">
+      <c r="E51" s="18">
         <f>SUM(B51:D51)/3</f>
         <v>4679.5</v>
       </c>
-      <c r="F51" s="23">
+      <c r="F51" s="21">
         <f t="shared" si="7"/>
         <v>1.05259233266076</v>
       </c>

</xml_diff>

<commit_message>
add meaningful message here
</commit_message>
<xml_diff>
--- a/Simulation & Risk/Data/Analysis_Data.xlsx
+++ b/Simulation & Risk/Data/Analysis_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Desktop\IAA\Spring 1\spring1-orange5\Simulation &amp; Risk\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k_cla\OneDrive\Desktop\MSA Program\spring1-orange5\Simulation &amp; Risk\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9C3C89-22BF-4998-AC44-FDCF3A7D2DF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC94E8D1-4372-4BF5-9D61-7131B1841177}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Projections" sheetId="1" r:id="rId1"/>
@@ -278,7 +278,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -307,18 +307,19 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -675,10 +676,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="23"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1152,10 +1153,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,16 +1176,16 @@
       <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
@@ -1202,7 +1203,7 @@
       <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="19" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1228,11 +1229,11 @@
       <c r="D4" s="11">
         <v>44</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="18">
         <f t="shared" ref="E4:E34" si="0">SUM(B4:D4)/3</f>
         <v>66.3</v>
       </c>
-      <c r="F4" s="22"/>
+      <c r="F4" s="20"/>
       <c r="G4" t="s">
         <v>13</v>
       </c>
@@ -1256,11 +1257,11 @@
       <c r="D5" s="13">
         <v>45.2</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="18">
         <f t="shared" si="0"/>
         <v>63.733333333333327</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="21">
         <f t="shared" ref="F5:F35" si="1">(E5-E4)/E4</f>
         <v>-3.8712921065862292E-2</v>
       </c>
@@ -1290,11 +1291,11 @@
       <c r="D6" s="14">
         <v>50.8</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <f t="shared" si="0"/>
         <v>67.366666666666674</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="21">
         <f t="shared" si="1"/>
         <v>5.7008368200837038E-2</v>
       </c>
@@ -1324,11 +1325,11 @@
       <c r="D7" s="13">
         <v>48.2</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="18">
         <f t="shared" si="0"/>
         <v>64.133333333333326</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="21">
         <f t="shared" si="1"/>
         <v>-4.7996041563582607E-2</v>
       </c>
@@ -1358,11 +1359,11 @@
       <c r="D8" s="14">
         <v>48.5</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="18">
         <f t="shared" si="0"/>
         <v>67.966666666666669</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="21">
         <f t="shared" si="1"/>
         <v>5.9771309771309927E-2</v>
       </c>
@@ -1392,11 +1393,11 @@
       <c r="D9" s="13">
         <v>53.1</v>
       </c>
-      <c r="E9" s="20">
+      <c r="E9" s="18">
         <f t="shared" si="0"/>
         <v>70.533333333333331</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="21">
         <f t="shared" si="1"/>
         <v>3.7763609612555114E-2</v>
       </c>
@@ -1426,11 +1427,11 @@
       <c r="D10" s="14">
         <v>56.9</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="18">
         <f t="shared" si="0"/>
         <v>84.3</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="21">
         <f t="shared" si="1"/>
         <v>0.19517958412098299</v>
       </c>
@@ -1460,11 +1461,11 @@
       <c r="D11" s="13">
         <v>61.5</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="18">
         <f t="shared" si="0"/>
         <v>89.7</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="21">
         <f t="shared" si="1"/>
         <v>6.4056939501779431E-2</v>
       </c>
@@ -1494,11 +1495,11 @@
       <c r="D12" s="14">
         <v>66.2</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="18">
         <f t="shared" si="0"/>
         <v>97.933333333333337</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="21">
         <f t="shared" si="1"/>
         <v>9.1787439613526575E-2</v>
       </c>
@@ -1528,11 +1529,11 @@
       <c r="D13" s="13">
         <v>70.2</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="18">
         <f t="shared" si="0"/>
         <v>103.66666666666667</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="21">
         <f t="shared" si="1"/>
         <v>5.8543226684819615E-2</v>
       </c>
@@ -1562,11 +1563,11 @@
       <c r="D14" s="14">
         <v>80.900000000000006</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="18">
         <f t="shared" si="0"/>
         <v>109.43333333333332</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="21">
         <f t="shared" si="1"/>
         <v>5.56270096463021E-2</v>
       </c>
@@ -1596,11 +1597,11 @@
       <c r="D15" s="13">
         <v>86.8</v>
       </c>
-      <c r="E15" s="20">
+      <c r="E15" s="18">
         <f t="shared" si="0"/>
         <v>110.60000000000001</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="21">
         <f t="shared" si="1"/>
         <v>1.0660980810234717E-2</v>
       </c>
@@ -1630,11 +1631,11 @@
       <c r="D16" s="14">
         <v>94.9</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="18">
         <f t="shared" si="0"/>
         <v>115.40000000000002</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="21">
         <f t="shared" si="1"/>
         <v>4.3399638336347295E-2</v>
       </c>
@@ -1664,11 +1665,11 @@
       <c r="D17" s="13">
         <v>105.8</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="18">
         <f t="shared" si="0"/>
         <v>121.63333333333334</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="21">
         <f t="shared" si="1"/>
         <v>5.4015020219526158E-2</v>
       </c>
@@ -1698,11 +1699,11 @@
       <c r="D18" s="14">
         <v>141.69999999999999</v>
       </c>
-      <c r="E18" s="20">
+      <c r="E18" s="18">
         <f t="shared" si="0"/>
         <v>147.03333333333333</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="21">
         <f t="shared" si="1"/>
         <v>0.20882433543436549</v>
       </c>
@@ -1732,11 +1733,11 @@
       <c r="D19" s="13">
         <v>177.2</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="18">
         <f t="shared" si="0"/>
         <v>192.6</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="21">
         <f t="shared" si="1"/>
         <v>0.30990705055542961</v>
       </c>
@@ -1766,11 +1767,11 @@
       <c r="D20" s="14">
         <v>190.3</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="18">
         <f t="shared" si="0"/>
         <v>203.93333333333331</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="21">
         <f t="shared" si="1"/>
         <v>5.8843890619591457E-2</v>
       </c>
@@ -1800,11 +1801,11 @@
       <c r="D21" s="13">
         <v>230.2</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="18">
         <f t="shared" si="0"/>
         <v>237.9</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="21">
         <f t="shared" si="1"/>
         <v>0.16655769859431205</v>
       </c>
@@ -1834,11 +1835,11 @@
       <c r="D22" s="14">
         <v>281.7</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="18">
         <f t="shared" si="0"/>
         <v>287.9666666666667</v>
       </c>
-      <c r="F22" s="23">
+      <c r="F22" s="21">
         <f t="shared" si="1"/>
         <v>0.21045257110830892</v>
       </c>
@@ -1868,11 +1869,11 @@
       <c r="D23" s="13">
         <v>339.6</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="18">
         <f t="shared" si="0"/>
         <v>341.93333333333339</v>
       </c>
-      <c r="F23" s="23">
+      <c r="F23" s="21">
         <f t="shared" si="1"/>
         <v>0.18740594976270411</v>
       </c>
@@ -1902,11 +1903,11 @@
       <c r="D24" s="14">
         <v>376.5</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="18">
         <f t="shared" si="0"/>
         <v>395</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="21">
         <f t="shared" si="1"/>
         <v>0.15519594462858236</v>
       </c>
@@ -1936,11 +1937,11 @@
       <c r="D25" s="13">
         <v>464</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="18">
         <f t="shared" si="0"/>
         <v>499.63333333333338</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="21">
         <f t="shared" si="1"/>
         <v>0.26489451476793263</v>
       </c>
@@ -1970,11 +1971,11 @@
       <c r="D26" s="14">
         <v>515.4</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="18">
         <f t="shared" si="0"/>
         <v>575.69999999999993</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="21">
         <f t="shared" si="1"/>
         <v>0.15224497965174436</v>
       </c>
@@ -2004,11 +2005,11 @@
       <c r="D27" s="13">
         <v>366.5</v>
       </c>
-      <c r="E27" s="20">
+      <c r="E27" s="18">
         <f t="shared" si="0"/>
         <v>419.4666666666667</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="21">
         <f t="shared" si="1"/>
         <v>-0.27137976955590282</v>
       </c>
@@ -2038,11 +2039,11 @@
       <c r="D28" s="14">
         <v>329.2</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="18">
         <f t="shared" si="0"/>
         <v>360.36666666666673</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="21">
         <f t="shared" si="1"/>
         <v>-0.14089319771137943</v>
       </c>
@@ -2072,11 +2073,11 @@
       <c r="D29" s="13">
         <v>372.3</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="18">
         <f t="shared" si="0"/>
         <v>383.79999999999995</v>
       </c>
-      <c r="F29" s="23">
+      <c r="F29" s="21">
         <f t="shared" si="1"/>
         <v>6.5026362038664007E-2</v>
       </c>
@@ -2106,11 +2107,11 @@
       <c r="D30" s="14">
         <v>389.2</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="18">
         <f t="shared" si="0"/>
         <v>399</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="21">
         <f t="shared" si="1"/>
         <v>3.9603960396039729E-2</v>
       </c>
@@ -2140,11 +2141,11 @@
       <c r="D31" s="13">
         <v>259.10000000000002</v>
       </c>
-      <c r="E31" s="20">
+      <c r="E31" s="18">
         <f t="shared" si="0"/>
         <v>295.16666666666669</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="21">
         <f t="shared" si="1"/>
         <v>-0.26023391812865493</v>
       </c>
@@ -2174,11 +2175,11 @@
       <c r="D32" s="14">
         <v>366.4</v>
       </c>
-      <c r="E32" s="20">
+      <c r="E32" s="18">
         <f t="shared" si="0"/>
         <v>368.7</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="21">
         <f t="shared" si="1"/>
         <v>0.24912478825522291</v>
       </c>
@@ -2208,11 +2209,11 @@
       <c r="D33" s="13">
         <v>355.4</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E33" s="18">
         <f t="shared" si="0"/>
         <v>365.16666666666669</v>
       </c>
-      <c r="F33" s="23">
+      <c r="F33" s="21">
         <f t="shared" si="1"/>
         <v>-9.5832203236596233E-3</v>
       </c>
@@ -2242,11 +2243,11 @@
       <c r="D34" s="14">
         <v>367.5</v>
       </c>
-      <c r="E34" s="20">
+      <c r="E34" s="18">
         <f t="shared" si="0"/>
         <v>386.86666666666662</v>
       </c>
-      <c r="F34" s="23">
+      <c r="F34" s="21">
         <f t="shared" si="1"/>
         <v>5.9424920127795336E-2</v>
       </c>
@@ -2276,11 +2277,11 @@
       <c r="D35" s="13">
         <v>441.2</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="18">
         <f>SUM(B35:D35)/3</f>
         <v>431.56666666666666</v>
       </c>
-      <c r="F35" s="23">
+      <c r="F35" s="21">
         <f t="shared" si="1"/>
         <v>0.11554368430122364</v>
       </c>
@@ -2310,11 +2311,11 @@
       <c r="D36" s="14">
         <v>357.6</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="18">
         <f t="shared" ref="E36:E49" si="6">SUM(B36:D36)/3</f>
         <v>382</v>
       </c>
-      <c r="F36" s="23">
+      <c r="F36" s="21">
         <f>(E36-E35)/E35</f>
         <v>-0.11485286166679538</v>
       </c>
@@ -2344,11 +2345,11 @@
       <c r="D37" s="13">
         <v>387.7</v>
       </c>
-      <c r="E37" s="20">
+      <c r="E37" s="18">
         <f t="shared" si="6"/>
         <v>421.83333333333331</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="21">
         <f t="shared" ref="F37:F51" si="7">(E37-E36)/E36</f>
         <v>0.10427574171029663</v>
       </c>
@@ -2378,11 +2379,11 @@
       <c r="D38" s="14">
         <v>491.5</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="18">
         <f t="shared" si="6"/>
         <v>478.7</v>
       </c>
-      <c r="F38" s="23">
+      <c r="F38" s="21">
         <f t="shared" si="7"/>
         <v>0.13480837613591468</v>
       </c>
@@ -2412,11 +2413,11 @@
       <c r="D39" s="13">
         <v>481.2</v>
       </c>
-      <c r="E39" s="20">
+      <c r="E39" s="18">
         <f t="shared" si="6"/>
         <v>508.90000000000003</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="21">
         <f t="shared" si="7"/>
         <v>6.3087528723626579E-2</v>
       </c>
@@ -2446,11 +2447,11 @@
       <c r="D40" s="14">
         <v>541</v>
       </c>
-      <c r="E40" s="20">
+      <c r="E40" s="18">
         <f t="shared" si="6"/>
         <v>499.33333333333331</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F40" s="21">
         <f t="shared" si="7"/>
         <v>-1.8798716185236233E-2</v>
       </c>
@@ -2480,11 +2481,11 @@
       <c r="D41" s="13">
         <v>655.6</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="18">
         <f t="shared" si="6"/>
         <v>609.93333333333339</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F41" s="21">
         <f t="shared" si="7"/>
         <v>0.2214953271028039</v>
       </c>
@@ -2514,11 +2515,11 @@
       <c r="D42" s="14">
         <v>973.2</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="18">
         <f t="shared" si="6"/>
         <v>784.93333333333339</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="21">
         <f t="shared" si="7"/>
         <v>0.28691660290742155</v>
       </c>
@@ -2548,11 +2549,11 @@
       <c r="D43" s="13">
         <v>1115.5</v>
       </c>
-      <c r="E43" s="20">
+      <c r="E43" s="18">
         <f t="shared" si="6"/>
         <v>898.9666666666667</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F43" s="21">
         <f t="shared" si="7"/>
         <v>0.14527773059283161</v>
       </c>
@@ -2582,11 +2583,11 @@
       <c r="D44" s="14">
         <v>1075.4000000000001</v>
       </c>
-      <c r="E44" s="20">
+      <c r="E44" s="18">
         <f t="shared" si="6"/>
         <v>808.56666666666661</v>
       </c>
-      <c r="F44" s="23">
+      <c r="F44" s="21">
         <f t="shared" si="7"/>
         <v>-0.1005599021098299</v>
       </c>
@@ -2616,11 +2617,11 @@
       <c r="D45" s="13">
         <v>1620.4</v>
       </c>
-      <c r="E45" s="20">
+      <c r="E45" s="18">
         <f t="shared" si="6"/>
         <v>1082</v>
       </c>
-      <c r="F45" s="23">
+      <c r="F45" s="21">
         <f t="shared" si="7"/>
         <v>0.33817042503194966</v>
       </c>
@@ -2650,11 +2651,11 @@
       <c r="D46" s="14">
         <v>1673.4</v>
       </c>
-      <c r="E46" s="20">
+      <c r="E46" s="18">
         <f t="shared" si="6"/>
         <v>1182.7</v>
       </c>
-      <c r="F46" s="23">
+      <c r="F46" s="21">
         <f t="shared" si="7"/>
         <v>9.3068391866913167E-2</v>
       </c>
@@ -2684,11 +2685,11 @@
       <c r="D47" s="13">
         <v>2065.1</v>
       </c>
-      <c r="E47" s="20">
+      <c r="E47" s="18">
         <f t="shared" si="6"/>
         <v>1402.8</v>
       </c>
-      <c r="F47" s="23">
+      <c r="F47" s="21">
         <f t="shared" si="7"/>
         <v>0.18609960260421063</v>
       </c>
@@ -2718,11 +2719,11 @@
       <c r="D48" s="14">
         <v>1977.3</v>
       </c>
-      <c r="E48" s="20">
+      <c r="E48" s="18">
         <f t="shared" si="6"/>
         <v>1711.8333333333333</v>
       </c>
-      <c r="F48" s="23">
+      <c r="F48" s="21">
         <f t="shared" si="7"/>
         <v>0.22029750023761999</v>
       </c>
@@ -2752,11 +2753,11 @@
       <c r="D49" s="13">
         <v>2392.9</v>
       </c>
-      <c r="E49" s="20">
+      <c r="E49" s="18">
         <f t="shared" si="6"/>
         <v>1936.9666666666665</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F49" s="21">
         <f t="shared" si="7"/>
         <v>0.13151591860578321</v>
       </c>
@@ -2786,11 +2787,11 @@
       <c r="D50" s="14">
         <v>2664.6</v>
       </c>
-      <c r="E50" s="20">
+      <c r="E50" s="18">
         <f>SUM(B50:D50)/3</f>
         <v>2279.7999999999997</v>
       </c>
-      <c r="F50" s="23">
+      <c r="F50" s="21">
         <f t="shared" si="7"/>
         <v>0.17699495775181123</v>
       </c>
@@ -2820,11 +2821,11 @@
       <c r="D51" s="13">
         <v>6131.2</v>
       </c>
-      <c r="E51" s="20">
+      <c r="E51" s="18">
         <f>SUM(B51:D51)/3</f>
         <v>4679.5</v>
       </c>
-      <c r="F51" s="23">
+      <c r="F51" s="21">
         <f t="shared" si="7"/>
         <v>1.05259233266076</v>
       </c>
@@ -2840,6 +2841,17 @@
         <f t="shared" si="5"/>
         <v>1.3009832620280717</v>
       </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G56" s="22"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H57" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>